<commit_message>
add sensor verify,tun zero. need debug
</commit_message>
<xml_diff>
--- a/01-22/addr.xlsx
+++ b/01-22/addr.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,18 +11,18 @@
   </sheets>
   <definedNames>
     <definedName name="变量名">Sheet1!$A:$A</definedName>
-    <definedName name="长度">Sheet1!$C:$C</definedName>
     <definedName name="地址">Sheet1!$B:$B</definedName>
     <definedName name="功能">Sheet1!$D:$D</definedName>
     <definedName name="宏名">Sheet1!$A:$A</definedName>
     <definedName name="页">Sheet1!$E:$E</definedName>
+    <definedName name="长度">Sheet1!$C:$C</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="735">
   <si>
     <t>0x0000</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2769,6 +2769,198 @@
   </si>
   <si>
     <t>0x0700</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOUCH_TUN_ZERO_BEGIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x706</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始调零</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOUCH_TUN_ZERO_END</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x707</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结束调零</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOUCH_TUN_ZERO_RETURN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x708</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调零界面返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_TUN_ZERO_CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x701</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调零界面CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_TUN_ZERO_HCHO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x705</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调零界面HCHO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_VERIFY_P_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x709</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的P0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_VERIFY_P_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_VERIFY_P_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_VERIFY_P_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_VERIFY_P_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_VERIFY_P_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_VERIFY_P_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_VERIFY_P_7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的P1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的P2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的P3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的P4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的P5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的P6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的P7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x70E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x713</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x718</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x71d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x722</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x727</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x72c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x731</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_VERIFY_VALUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的校准值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDR_REAL_VALUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x736</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的实际值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOUCH_VERIFY_EXIT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x737</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校准界面的推出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2900,14 +3092,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="ECE9D8"/>
+        <a:sysClr val="window" lastClr="A0A0A4"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2942,7 +3134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2977,7 +3169,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3186,10 +3378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E253"/>
+  <dimension ref="A1:E271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
+      <selection activeCell="C267" sqref="C267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7108,6 +7300,278 @@
         <v>35</v>
       </c>
     </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A255" t="s">
+        <v>687</v>
+      </c>
+      <c r="B255" t="s">
+        <v>688</v>
+      </c>
+      <c r="C255">
+        <v>0</v>
+      </c>
+      <c r="D255" t="s">
+        <v>689</v>
+      </c>
+      <c r="E255">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A256" t="s">
+        <v>690</v>
+      </c>
+      <c r="B256" t="s">
+        <v>691</v>
+      </c>
+      <c r="C256">
+        <v>0</v>
+      </c>
+      <c r="D256" t="s">
+        <v>692</v>
+      </c>
+      <c r="E256">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A257" t="s">
+        <v>693</v>
+      </c>
+      <c r="B257" t="s">
+        <v>694</v>
+      </c>
+      <c r="C257">
+        <v>0</v>
+      </c>
+      <c r="D257" t="s">
+        <v>695</v>
+      </c>
+      <c r="E257">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A258" t="s">
+        <v>696</v>
+      </c>
+      <c r="B258" t="s">
+        <v>697</v>
+      </c>
+      <c r="C258">
+        <v>4</v>
+      </c>
+      <c r="D258" t="s">
+        <v>698</v>
+      </c>
+      <c r="E258">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A259" t="s">
+        <v>699</v>
+      </c>
+      <c r="B259" t="s">
+        <v>700</v>
+      </c>
+      <c r="C259">
+        <v>4</v>
+      </c>
+      <c r="D259" t="s">
+        <v>701</v>
+      </c>
+      <c r="E259">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A261" t="s">
+        <v>702</v>
+      </c>
+      <c r="B261" t="s">
+        <v>703</v>
+      </c>
+      <c r="C261">
+        <v>5</v>
+      </c>
+      <c r="D261" t="s">
+        <v>704</v>
+      </c>
+      <c r="E261">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A262" t="s">
+        <v>705</v>
+      </c>
+      <c r="B262" t="s">
+        <v>719</v>
+      </c>
+      <c r="C262">
+        <v>5</v>
+      </c>
+      <c r="D262" t="s">
+        <v>712</v>
+      </c>
+      <c r="E262">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A263" t="s">
+        <v>706</v>
+      </c>
+      <c r="B263" t="s">
+        <v>720</v>
+      </c>
+      <c r="C263">
+        <v>5</v>
+      </c>
+      <c r="D263" t="s">
+        <v>713</v>
+      </c>
+      <c r="E263">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A264" t="s">
+        <v>707</v>
+      </c>
+      <c r="B264" t="s">
+        <v>721</v>
+      </c>
+      <c r="C264">
+        <v>5</v>
+      </c>
+      <c r="D264" t="s">
+        <v>714</v>
+      </c>
+      <c r="E264">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A265" t="s">
+        <v>708</v>
+      </c>
+      <c r="B265" t="s">
+        <v>722</v>
+      </c>
+      <c r="C265">
+        <v>5</v>
+      </c>
+      <c r="D265" t="s">
+        <v>715</v>
+      </c>
+      <c r="E265">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A266" t="s">
+        <v>709</v>
+      </c>
+      <c r="B266" t="s">
+        <v>723</v>
+      </c>
+      <c r="C266">
+        <v>5</v>
+      </c>
+      <c r="D266" t="s">
+        <v>716</v>
+      </c>
+      <c r="E266">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A267" t="s">
+        <v>710</v>
+      </c>
+      <c r="B267" t="s">
+        <v>724</v>
+      </c>
+      <c r="C267">
+        <v>5</v>
+      </c>
+      <c r="D267" t="s">
+        <v>717</v>
+      </c>
+      <c r="E267">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A268" t="s">
+        <v>711</v>
+      </c>
+      <c r="B268" t="s">
+        <v>725</v>
+      </c>
+      <c r="C268">
+        <v>5</v>
+      </c>
+      <c r="D268" t="s">
+        <v>718</v>
+      </c>
+      <c r="E268">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A269" t="s">
+        <v>727</v>
+      </c>
+      <c r="B269" t="s">
+        <v>726</v>
+      </c>
+      <c r="C269">
+        <v>5</v>
+      </c>
+      <c r="D269" t="s">
+        <v>728</v>
+      </c>
+      <c r="E269">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A270" t="s">
+        <v>729</v>
+      </c>
+      <c r="B270" t="s">
+        <v>730</v>
+      </c>
+      <c r="C270">
+        <v>5</v>
+      </c>
+      <c r="D270" t="s">
+        <v>731</v>
+      </c>
+      <c r="E270">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A271" t="s">
+        <v>732</v>
+      </c>
+      <c r="B271" t="s">
+        <v>733</v>
+      </c>
+      <c r="C271">
+        <v>0</v>
+      </c>
+      <c r="D271" t="s">
+        <v>734</v>
+      </c>
+      <c r="E271">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>